<commit_message>
test new layer and set verbose to true
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -474,11 +474,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3.2</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="3">
@@ -495,11 +495,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2.9</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="4">
@@ -516,11 +516,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="5">
@@ -537,11 +537,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>3.1</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="6">
@@ -558,11 +558,11 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>3.3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -579,11 +579,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>3.2</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="8">
@@ -600,11 +600,11 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="9">
@@ -621,11 +621,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3.4</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="10">
@@ -642,11 +642,11 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2.8</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="11">
@@ -663,11 +663,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>3.5</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="12">
@@ -684,11 +684,11 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>2.71</v>
+        <v>2.91</v>
       </c>
     </row>
     <row r="13">
@@ -705,11 +705,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2.32</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="14">
@@ -726,11 +726,11 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>2.18</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="15">
@@ -747,11 +747,11 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>2.07</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="16">
@@ -768,11 +768,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>1.88</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="17">
@@ -789,11 +789,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>2.22</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="18">
@@ -810,11 +810,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2.13</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="19">
@@ -831,11 +831,11 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>2.11</v>
+        <v>2.93</v>
       </c>
     </row>
     <row r="20">
@@ -852,11 +852,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>2.06</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="21">
@@ -873,11 +873,11 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>2.28</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="22">
@@ -894,11 +894,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>2.1</v>
+        <v>3.37</v>
       </c>
     </row>
     <row r="23">
@@ -915,11 +915,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>2.04</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="24">
@@ -936,11 +936,11 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>2.12</v>
+        <v>2.86</v>
       </c>
     </row>
     <row r="25">
@@ -957,11 +957,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>1.67</v>
+        <v>2.99</v>
       </c>
     </row>
     <row r="26">
@@ -978,11 +978,11 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>2.48</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="27">
@@ -999,11 +999,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>1.95</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="28">
@@ -1020,11 +1020,11 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>2.71</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="29">
@@ -1041,11 +1041,11 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>2.33</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="30">
@@ -1062,11 +1062,11 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>2.32</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="31">
@@ -1083,11 +1083,11 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>黄土</t>
+          <t>粉土</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>2.6</v>
+        <v>2.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>